<commit_message>
SSDM-10984 : Test Fix+Improving error messages
</commit_message>
<xml_diff>
--- a/openbis_standard_technologies/sourceTest/java/ch/ethz/sis/openbis/systemtest/plugin/excelimport/test_files/samples/general_eln_settings_update.xlsx
+++ b/openbis_standard_technologies/sourceTest/java/ch/ethz/sis/openbis/systemtest/plugin/excelimport/test_files/samples/general_eln_settings_update.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariapukhliakova/git/openbis/openbis_standard_technologies/sourceTest/java/ch/ethz/sis/openbis/systemtest/plugin/excelimport/test_files/samples/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juanf/Documents/sissource/openbis/openbis_standard_technologies/sourceTest/java/ch/ethz/sis/openbis/systemtest/plugin/excelimport/test_files/samples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE511E22-5D97-1240-9786-3AB3448AA893}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C660E23-4439-9744-88F1-9F5480C888B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5960" yWindow="460" windowWidth="27640" windowHeight="19120" xr2:uid="{2B43D852-C8D1-EE49-967E-9FF3E3EA802A}"/>
+    <workbookView xWindow="-34960" yWindow="4180" windowWidth="27640" windowHeight="19120" xr2:uid="{2B43D852-C8D1-EE49-967E-9FF3E3EA802A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
   <si>
     <t>SAMPLE</t>
   </si>
@@ -94,13 +94,22 @@
   </si>
   <si>
     <t>Default Experiment Updated</t>
+  </si>
+  <si>
+    <t>Identifier</t>
+  </si>
+  <si>
+    <t>/ELN_SETTINGS/DEFAULT_PROJECT/DEFAULT_EXPERIMENT</t>
+  </si>
+  <si>
+    <t>/ELN_SETTINGS/GENERAL_ELN_SETTINGS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -136,6 +145,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -157,7 +174,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -171,6 +188,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -485,26 +503,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{138B54B5-3BF8-0D42-A5D4-7E41A9E763E6}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="22.33203125" customWidth="1"/>
-    <col min="2" max="2" width="29.6640625" customWidth="1"/>
+    <col min="1" max="1" width="52" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17">
+    <row r="1" spans="1:4" ht="17">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B1" s="2"/>
     </row>
-    <row r="2" spans="1:3" ht="17">
+    <row r="2" spans="1:4" ht="17">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -512,7 +530,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -520,113 +538,131 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="17">
+    <row r="5" spans="1:4" ht="17">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:3" ht="17">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:4" ht="17">
+      <c r="A6" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:4">
       <c r="A7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="17">
+    <row r="9" spans="1:4" ht="17">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B9" s="2"/>
     </row>
-    <row r="10" spans="1:3" ht="17">
+    <row r="10" spans="1:4" ht="17">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
     </row>
-    <row r="12" spans="1:3" ht="17">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:4" ht="17">
+      <c r="A12" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="D12" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:4">
       <c r="A13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="17">
+    <row r="15" spans="1:4" ht="17">
       <c r="A15" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B15" s="2"/>
     </row>
-    <row r="16" spans="1:3" ht="17">
+    <row r="16" spans="1:4" ht="17">
       <c r="A16" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="17">
-      <c r="A18" s="3" t="s">
+    <row r="18" spans="1:4" ht="17">
+      <c r="A18" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="D18" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:4">
       <c r="A19" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="C19" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="D19" s="5" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>